<commit_message>
Update Geral + Add MyProcessor
</commit_message>
<xml_diff>
--- a/spring-batch-training/MyKnowledge.xlsx
+++ b/spring-batch-training/MyKnowledge.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adriano\Desktop\SpringToolProject\WorkWithJobsAndSteps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adriano\git\spring-batch-training\spring-batch-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273EEA42-3459-4865-A7E0-F36C0E5A2169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDF0B7-F8D8-4241-8AC1-C70FC0CE4853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23400" yWindow="6444" windowWidth="17556" windowHeight="15960" xr2:uid="{6B6D4B2B-ACC6-4399-A668-F7F9AF4731BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Job</t>
   </si>
@@ -74,12 +74,24 @@
   <si>
     <t>JSONData</t>
   </si>
+  <si>
+    <t>ValidatingItemProcessor</t>
+  </si>
+  <si>
+    <t>ScriptItemProcessor</t>
+  </si>
+  <si>
+    <t>CompositeItemProcessor</t>
+  </si>
+  <si>
+    <t>ClassifierCompositeItemProcessor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +109,12 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -242,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -309,6 +327,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,12 +405,12 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>198120</xdr:rowOff>
     </xdr:to>
@@ -408,8 +427,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3192780" y="2141220"/>
-          <a:ext cx="1691640" cy="3169920"/>
+          <a:off x="3192780" y="2423160"/>
+          <a:ext cx="1417320" cy="2887980"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -831,10 +850,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
@@ -855,8 +874,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5036820" y="2156460"/>
-          <a:ext cx="434340" cy="1082040"/>
+          <a:off x="4869180" y="2354580"/>
+          <a:ext cx="601980" cy="883920"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -916,6 +935,288 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector de Seta Reta 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B7616D5-52E4-4A82-B0C0-28B8A663E118}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5798820" y="2209800"/>
+          <a:ext cx="807720" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector de Seta Reta 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234AF0BD-FA29-4F77-A500-095AC8980D0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6934200" y="548640"/>
+          <a:ext cx="1485900" cy="830580"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector de Seta Reta 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E6CD93-1C7D-4D5C-B639-6BA75A9DB051}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6911340" y="1356360"/>
+          <a:ext cx="1531620" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector de Seta Reta 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BBD0414-4DFE-4BAF-9E47-769803215C08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6896100" y="2011680"/>
+          <a:ext cx="1516380" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector de Seta Reta 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA927E9-8D1A-40BB-9B6A-C52DCCFE4CD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6972300" y="2354580"/>
+          <a:ext cx="1379220" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
           <a:prstDash val="sysDot"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -1237,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1A0DF4-BEBC-4AD8-B734-01DFE2C1CA1A}">
-  <dimension ref="B1:AE26"/>
+  <dimension ref="B1:AO26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -1249,8 +1550,8 @@
     <col min="80" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B2" s="57" t="s">
         <v>10</v>
       </c>
@@ -1277,8 +1578,17 @@
       <c r="AC2" s="49"/>
       <c r="AD2" s="49"/>
       <c r="AE2" s="50"/>
-    </row>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG2" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="59"/>
+    </row>
+    <row r="3" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B3" s="60"/>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -1303,8 +1613,15 @@
       <c r="AC3" s="41"/>
       <c r="AD3" s="42"/>
       <c r="AE3" s="52"/>
-    </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG3" s="63"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="65"/>
+    </row>
+    <row r="4" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B4" s="60"/>
       <c r="C4" s="61"/>
       <c r="D4" s="61"/>
@@ -1330,7 +1647,7 @@
       <c r="AD4" s="44"/>
       <c r="AE4" s="52"/>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B5" s="63"/>
       <c r="C5" s="64"/>
       <c r="D5" s="64"/>
@@ -1355,8 +1672,17 @@
       <c r="AC5" s="35"/>
       <c r="AD5" s="44"/>
       <c r="AE5" s="52"/>
-    </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG5" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58"/>
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="59"/>
+    </row>
+    <row r="6" spans="2:41" x14ac:dyDescent="0.35">
       <c r="N6" s="51"/>
       <c r="O6" s="43"/>
       <c r="P6" s="33"/>
@@ -1377,8 +1703,15 @@
       <c r="AC6" s="35"/>
       <c r="AD6" s="44"/>
       <c r="AE6" s="52"/>
-    </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG6" s="63"/>
+      <c r="AH6" s="64"/>
+      <c r="AI6" s="64"/>
+      <c r="AJ6" s="64"/>
+      <c r="AK6" s="64"/>
+      <c r="AL6" s="64"/>
+      <c r="AM6" s="65"/>
+    </row>
+    <row r="7" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B7" s="57" t="s">
         <v>11</v>
       </c>
@@ -1404,7 +1737,7 @@
       <c r="AD7" s="44"/>
       <c r="AE7" s="52"/>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B8" s="60"/>
       <c r="C8" s="61"/>
       <c r="D8" s="61"/>
@@ -1427,8 +1760,17 @@
       <c r="AC8" s="35"/>
       <c r="AD8" s="44"/>
       <c r="AE8" s="52"/>
-    </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG8" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH8" s="58"/>
+      <c r="AI8" s="58"/>
+      <c r="AJ8" s="58"/>
+      <c r="AK8" s="58"/>
+      <c r="AL8" s="58"/>
+      <c r="AM8" s="59"/>
+    </row>
+    <row r="9" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B9" s="60"/>
       <c r="C9" s="61"/>
       <c r="D9" s="61"/>
@@ -1451,8 +1793,15 @@
       <c r="AC9" s="35"/>
       <c r="AD9" s="44"/>
       <c r="AE9" s="52"/>
-    </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG9" s="63"/>
+      <c r="AH9" s="64"/>
+      <c r="AI9" s="64"/>
+      <c r="AJ9" s="64"/>
+      <c r="AK9" s="64"/>
+      <c r="AL9" s="64"/>
+      <c r="AM9" s="65"/>
+    </row>
+    <row r="10" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B10" s="63"/>
       <c r="C10" s="64"/>
       <c r="D10" s="64"/>
@@ -1476,7 +1825,7 @@
       <c r="AD10" s="44"/>
       <c r="AE10" s="52"/>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:41" x14ac:dyDescent="0.35">
       <c r="G11" s="2"/>
       <c r="N11" s="51"/>
       <c r="O11" s="43"/>
@@ -1496,8 +1845,19 @@
       <c r="AC11" s="35"/>
       <c r="AD11" s="44"/>
       <c r="AE11" s="52"/>
-    </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG11" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH11" s="58"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AK11" s="58"/>
+      <c r="AL11" s="58"/>
+      <c r="AM11" s="58"/>
+      <c r="AN11" s="58"/>
+      <c r="AO11" s="59"/>
+    </row>
+    <row r="12" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B12" s="57" t="s">
         <v>12</v>
       </c>
@@ -1525,8 +1885,17 @@
       <c r="AC12" s="35"/>
       <c r="AD12" s="44"/>
       <c r="AE12" s="52"/>
-    </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="AG12" s="63"/>
+      <c r="AH12" s="64"/>
+      <c r="AI12" s="64"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="64"/>
+      <c r="AL12" s="64"/>
+      <c r="AM12" s="64"/>
+      <c r="AN12" s="64"/>
+      <c r="AO12" s="65"/>
+    </row>
+    <row r="13" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B13" s="60"/>
       <c r="C13" s="61"/>
       <c r="D13" s="61"/>
@@ -1551,7 +1920,7 @@
       <c r="AD13" s="44"/>
       <c r="AE13" s="52"/>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B14" s="60"/>
       <c r="C14" s="61"/>
       <c r="D14" s="61"/>
@@ -1576,7 +1945,7 @@
       <c r="AD14" s="44"/>
       <c r="AE14" s="52"/>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:41" x14ac:dyDescent="0.35">
       <c r="B15" s="63"/>
       <c r="C15" s="64"/>
       <c r="D15" s="64"/>
@@ -1601,7 +1970,7 @@
       <c r="AD15" s="44"/>
       <c r="AE15" s="52"/>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.35">
       <c r="G16" s="2"/>
       <c r="N16" s="51"/>
       <c r="O16" s="43"/>

</xml_diff>

<commit_message>
Various Refactor - Update MyWriter And MyStepChunk
</commit_message>
<xml_diff>
--- a/spring-batch-training/MyKnowledge.xlsx
+++ b/spring-batch-training/MyKnowledge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adriano\git\spring-batch-training\spring-batch-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDF0B7-F8D8-4241-8AC1-C70FC0CE4853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7237CC20-8719-490F-980D-8D2ED4797607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23400" yWindow="6444" windowWidth="17556" windowHeight="15960" xr2:uid="{6B6D4B2B-ACC6-4399-A668-F7F9AF4731BC}"/>
+    <workbookView xWindow="9552" yWindow="3900" windowWidth="17556" windowHeight="15960" xr2:uid="{6B6D4B2B-ACC6-4399-A668-F7F9AF4731BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Job</t>
   </si>
@@ -86,12 +86,36 @@
   <si>
     <t>ClassifierCompositeItemProcessor</t>
   </si>
+  <si>
+    <t>GrupoLancamento</t>
+  </si>
+  <si>
+    <t>Bean</t>
+  </si>
+  <si>
+    <t>MyJdbcItemReader</t>
+  </si>
+  <si>
+    <t>JdbcCursorItemReaderConfig</t>
+  </si>
+  <si>
+    <t>JdbcCursorItemReader</t>
+  </si>
+  <si>
+    <t>MultiResourceItemReader</t>
+  </si>
+  <si>
+    <t>FlatFileItemReader</t>
+  </si>
+  <si>
+    <t>FlatFileItemReaderConfig</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +141,33 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -328,6 +383,50 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,6 +1315,342 @@
         <a:ln w="38100">
           <a:solidFill>
             <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector de Seta Reta 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB71C64-D5F3-41B1-954B-ED9EFB2A9235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4899660" y="9585960"/>
+          <a:ext cx="1432560" cy="1051560"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Conector de Seta Reta 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B00B22-453A-498E-93B7-9072CAA17640}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="8633460"/>
+          <a:ext cx="2918460" cy="586740"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector de Seta Reta 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDB54BCA-34F1-4528-B43B-4E733B1DEFCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1577340" y="9654540"/>
+          <a:ext cx="2750820" cy="1021080"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector de Seta Reta 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{816E9146-F674-44D4-96E6-7522109E177E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4899660" y="9585960"/>
+          <a:ext cx="1432560" cy="1051560"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector de Seta Reta 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946E6AED-6E0A-4CE0-B45F-E62285013242}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="8633460"/>
+          <a:ext cx="2918460" cy="586740"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector de Seta Reta 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B324977-5845-4610-9C50-5D3D871E6460}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1577340" y="9654540"/>
+          <a:ext cx="2750820" cy="1021080"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
           </a:solidFill>
           <a:prstDash val="sysDot"/>
           <a:tailEnd type="triangle"/>
@@ -1538,10 +1973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1A0DF4-BEBC-4AD8-B734-01DFE2C1CA1A}">
-  <dimension ref="B1:AO26"/>
+  <dimension ref="B1:AO64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="AI49" sqref="AI49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2145,7 +2580,884 @@
       <c r="AB26" s="54"/>
       <c r="AC26" s="55"/>
     </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="M30" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="49"/>
+      <c r="V30" s="49"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="49"/>
+      <c r="Y30" s="49"/>
+      <c r="Z30" s="49"/>
+      <c r="AA30" s="49"/>
+      <c r="AB30" s="49"/>
+      <c r="AC30" s="49"/>
+      <c r="AD30" s="50"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="M31" s="51"/>
+      <c r="N31" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
+      <c r="V31" s="41"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="41"/>
+      <c r="AA31" s="41"/>
+      <c r="AB31" s="41"/>
+      <c r="AC31" s="42"/>
+      <c r="AD31" s="52"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.35">
+      <c r="D32" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="79"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="31"/>
+      <c r="AA32" s="31"/>
+      <c r="AB32" s="32"/>
+      <c r="AC32" s="44"/>
+      <c r="AD32" s="52"/>
+    </row>
+    <row r="33" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="34"/>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="39"/>
+      <c r="Z33" s="39"/>
+      <c r="AA33" s="39"/>
+      <c r="AB33" s="35"/>
+      <c r="AC33" s="44"/>
+      <c r="AD33" s="52"/>
+    </row>
+    <row r="34" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D34" s="75"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="76"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+      <c r="AA34" s="39"/>
+      <c r="AB34" s="35"/>
+      <c r="AC34" s="44"/>
+      <c r="AD34" s="52"/>
+    </row>
+    <row r="35" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D35" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="76"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="39"/>
+      <c r="W35" s="39"/>
+      <c r="X35" s="39"/>
+      <c r="Y35" s="39"/>
+      <c r="Z35" s="39"/>
+      <c r="AA35" s="39"/>
+      <c r="AB35" s="35"/>
+      <c r="AC35" s="44"/>
+      <c r="AD35" s="52"/>
+    </row>
+    <row r="36" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D36" s="68"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="39"/>
+      <c r="W36" s="39"/>
+      <c r="X36" s="39"/>
+      <c r="Y36" s="39"/>
+      <c r="Z36" s="39"/>
+      <c r="AA36" s="39"/>
+      <c r="AB36" s="35"/>
+      <c r="AC36" s="44"/>
+      <c r="AD36" s="52"/>
+    </row>
+    <row r="37" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D37" s="71"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="73"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q37" s="84"/>
+      <c r="R37" s="84"/>
+      <c r="S37" s="84"/>
+      <c r="T37" s="84"/>
+      <c r="U37" s="85"/>
+      <c r="V37" s="39"/>
+      <c r="W37" s="39"/>
+      <c r="X37" s="39"/>
+      <c r="Y37" s="39"/>
+      <c r="Z37" s="39"/>
+      <c r="AA37" s="39"/>
+      <c r="AB37" s="35"/>
+      <c r="AC37" s="44"/>
+      <c r="AD37" s="52"/>
+    </row>
+    <row r="38" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M38" s="51"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="39"/>
+      <c r="W38" s="39"/>
+      <c r="X38" s="39"/>
+      <c r="Y38" s="39"/>
+      <c r="Z38" s="39"/>
+      <c r="AA38" s="39"/>
+      <c r="AB38" s="35"/>
+      <c r="AC38" s="44"/>
+      <c r="AD38" s="52"/>
+    </row>
+    <row r="39" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D39" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="82"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="34"/>
+      <c r="W39" s="34"/>
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="35"/>
+      <c r="AC39" s="44"/>
+      <c r="AD39" s="52"/>
+    </row>
+    <row r="40" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D40" s="68"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="70"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="34"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="34"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y40" s="22"/>
+      <c r="Z40" s="22"/>
+      <c r="AA40" s="23"/>
+      <c r="AB40" s="35"/>
+      <c r="AC40" s="44"/>
+      <c r="AD40" s="52"/>
+    </row>
+    <row r="41" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D41" s="75"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="76"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="34"/>
+      <c r="Q41" s="34"/>
+      <c r="R41" s="34"/>
+      <c r="S41" s="34"/>
+      <c r="T41" s="34"/>
+      <c r="U41" s="34"/>
+      <c r="V41" s="34"/>
+      <c r="W41" s="34"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="25"/>
+      <c r="Z41" s="25"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="35"/>
+      <c r="AC41" s="44"/>
+      <c r="AD41" s="52"/>
+    </row>
+    <row r="42" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D42" s="75"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="76"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="34"/>
+      <c r="T42" s="34"/>
+      <c r="U42" s="34"/>
+      <c r="V42" s="34"/>
+      <c r="W42" s="34"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="25"/>
+      <c r="Z42" s="25"/>
+      <c r="AA42" s="26"/>
+      <c r="AB42" s="35"/>
+      <c r="AC42" s="44"/>
+      <c r="AD42" s="52"/>
+    </row>
+    <row r="43" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="70"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="34"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="34"/>
+      <c r="S43" s="34"/>
+      <c r="T43" s="34"/>
+      <c r="U43" s="34"/>
+      <c r="V43" s="34"/>
+      <c r="W43" s="34"/>
+      <c r="X43" s="27"/>
+      <c r="Y43" s="28"/>
+      <c r="Z43" s="28"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="35"/>
+      <c r="AC43" s="44"/>
+      <c r="AD43" s="52"/>
+    </row>
+    <row r="44" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D44" s="71"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="73"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="36"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="37"/>
+      <c r="V44" s="37"/>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="37"/>
+      <c r="AA44" s="37"/>
+      <c r="AB44" s="38"/>
+      <c r="AC44" s="44"/>
+      <c r="AD44" s="52"/>
+    </row>
+    <row r="45" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M45" s="51"/>
+      <c r="N45" s="45"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="46"/>
+      <c r="T45" s="46"/>
+      <c r="U45" s="46"/>
+      <c r="V45" s="46"/>
+      <c r="W45" s="46"/>
+      <c r="X45" s="46"/>
+      <c r="Y45" s="46"/>
+      <c r="Z45" s="46"/>
+      <c r="AA45" s="46"/>
+      <c r="AB45" s="46"/>
+      <c r="AC45" s="47"/>
+      <c r="AD45" s="52"/>
+    </row>
+    <row r="46" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M46" s="53"/>
+      <c r="N46" s="54"/>
+      <c r="O46" s="54"/>
+      <c r="P46" s="54"/>
+      <c r="Q46" s="54"/>
+      <c r="R46" s="54"/>
+      <c r="S46" s="54"/>
+      <c r="T46" s="54"/>
+      <c r="U46" s="54"/>
+      <c r="V46" s="54"/>
+      <c r="W46" s="54"/>
+      <c r="X46" s="54"/>
+      <c r="Y46" s="54"/>
+      <c r="Z46" s="54"/>
+      <c r="AA46" s="54"/>
+      <c r="AB46" s="54"/>
+      <c r="AC46" s="54"/>
+      <c r="AD46" s="55"/>
+    </row>
+    <row r="48" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M48" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49"/>
+      <c r="Q48" s="49"/>
+      <c r="R48" s="49"/>
+      <c r="S48" s="49"/>
+      <c r="T48" s="49"/>
+      <c r="U48" s="49"/>
+      <c r="V48" s="49"/>
+      <c r="W48" s="49"/>
+      <c r="X48" s="49"/>
+      <c r="Y48" s="49"/>
+      <c r="Z48" s="49"/>
+      <c r="AA48" s="49"/>
+      <c r="AB48" s="49"/>
+      <c r="AC48" s="49"/>
+      <c r="AD48" s="50"/>
+    </row>
+    <row r="49" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="K49" s="86"/>
+      <c r="M49" s="51"/>
+      <c r="N49" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="O49" s="41"/>
+      <c r="P49" s="41"/>
+      <c r="Q49" s="41"/>
+      <c r="R49" s="41"/>
+      <c r="S49" s="41"/>
+      <c r="T49" s="41"/>
+      <c r="U49" s="41"/>
+      <c r="V49" s="41"/>
+      <c r="W49" s="41"/>
+      <c r="X49" s="41"/>
+      <c r="Y49" s="41"/>
+      <c r="Z49" s="41"/>
+      <c r="AA49" s="41"/>
+      <c r="AB49" s="41"/>
+      <c r="AC49" s="42"/>
+      <c r="AD49" s="52"/>
+    </row>
+    <row r="50" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D50" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="78"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="79"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="43"/>
+      <c r="O50" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
+      <c r="S50" s="31"/>
+      <c r="T50" s="31"/>
+      <c r="U50" s="31"/>
+      <c r="V50" s="31"/>
+      <c r="W50" s="31"/>
+      <c r="X50" s="31"/>
+      <c r="Y50" s="31"/>
+      <c r="Z50" s="31"/>
+      <c r="AA50" s="31"/>
+      <c r="AB50" s="32"/>
+      <c r="AC50" s="44"/>
+      <c r="AD50" s="52"/>
+    </row>
+    <row r="51" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D51" s="68"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="70"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="43"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="34"/>
+      <c r="Q51" s="34"/>
+      <c r="R51" s="34"/>
+      <c r="S51" s="34"/>
+      <c r="T51" s="34"/>
+      <c r="U51" s="34"/>
+      <c r="V51" s="39"/>
+      <c r="W51" s="39"/>
+      <c r="X51" s="39"/>
+      <c r="Y51" s="39"/>
+      <c r="Z51" s="39"/>
+      <c r="AA51" s="39"/>
+      <c r="AB51" s="35"/>
+      <c r="AC51" s="44"/>
+      <c r="AD51" s="52"/>
+    </row>
+    <row r="52" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D52" s="75"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="76"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="43"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="39"/>
+      <c r="W52" s="39"/>
+      <c r="X52" s="39"/>
+      <c r="Y52" s="39"/>
+      <c r="Z52" s="39"/>
+      <c r="AA52" s="39"/>
+      <c r="AB52" s="35"/>
+      <c r="AC52" s="44"/>
+      <c r="AD52" s="52"/>
+    </row>
+    <row r="53" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D53" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
+      <c r="H53" s="74"/>
+      <c r="I53" s="76"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="43"/>
+      <c r="O53" s="33"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="39"/>
+      <c r="W53" s="39"/>
+      <c r="X53" s="39"/>
+      <c r="Y53" s="39"/>
+      <c r="Z53" s="39"/>
+      <c r="AA53" s="39"/>
+      <c r="AB53" s="35"/>
+      <c r="AC53" s="44"/>
+      <c r="AD53" s="52"/>
+    </row>
+    <row r="54" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D54" s="68"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
+      <c r="I54" s="70"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="43"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="39"/>
+      <c r="W54" s="39"/>
+      <c r="X54" s="39"/>
+      <c r="Y54" s="39"/>
+      <c r="Z54" s="39"/>
+      <c r="AA54" s="39"/>
+      <c r="AB54" s="35"/>
+      <c r="AC54" s="44"/>
+      <c r="AD54" s="52"/>
+    </row>
+    <row r="55" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D55" s="71"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="72"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="73"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="33"/>
+      <c r="P55" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q55" s="84"/>
+      <c r="R55" s="84"/>
+      <c r="S55" s="84"/>
+      <c r="T55" s="84"/>
+      <c r="U55" s="85"/>
+      <c r="V55" s="39"/>
+      <c r="W55" s="39"/>
+      <c r="X55" s="39"/>
+      <c r="Y55" s="39"/>
+      <c r="Z55" s="39"/>
+      <c r="AA55" s="39"/>
+      <c r="AB55" s="35"/>
+      <c r="AC55" s="44"/>
+      <c r="AD55" s="52"/>
+    </row>
+    <row r="56" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M56" s="51"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="33"/>
+      <c r="P56" s="6"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="39"/>
+      <c r="W56" s="39"/>
+      <c r="X56" s="39"/>
+      <c r="Y56" s="39"/>
+      <c r="Z56" s="39"/>
+      <c r="AA56" s="39"/>
+      <c r="AB56" s="35"/>
+      <c r="AC56" s="44"/>
+      <c r="AD56" s="52"/>
+    </row>
+    <row r="57" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D57" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="81"/>
+      <c r="F57" s="81"/>
+      <c r="G57" s="81"/>
+      <c r="H57" s="81"/>
+      <c r="I57" s="82"/>
+      <c r="M57" s="51"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="33"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="10"/>
+      <c r="U57" s="11"/>
+      <c r="V57" s="34"/>
+      <c r="W57" s="34"/>
+      <c r="X57" s="34"/>
+      <c r="Y57" s="34"/>
+      <c r="Z57" s="34"/>
+      <c r="AA57" s="34"/>
+      <c r="AB57" s="35"/>
+      <c r="AC57" s="44"/>
+      <c r="AD57" s="52"/>
+    </row>
+    <row r="58" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D58" s="68"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="70"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="33"/>
+      <c r="P58" s="34"/>
+      <c r="Q58" s="34"/>
+      <c r="R58" s="34"/>
+      <c r="S58" s="34"/>
+      <c r="T58" s="34"/>
+      <c r="U58" s="34"/>
+      <c r="V58" s="34"/>
+      <c r="W58" s="34"/>
+      <c r="X58" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y58" s="22"/>
+      <c r="Z58" s="22"/>
+      <c r="AA58" s="23"/>
+      <c r="AB58" s="35"/>
+      <c r="AC58" s="44"/>
+      <c r="AD58" s="52"/>
+    </row>
+    <row r="59" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D59" s="75"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="76"/>
+      <c r="M59" s="51"/>
+      <c r="N59" s="43"/>
+      <c r="O59" s="33"/>
+      <c r="P59" s="34"/>
+      <c r="Q59" s="34"/>
+      <c r="R59" s="34"/>
+      <c r="S59" s="34"/>
+      <c r="T59" s="34"/>
+      <c r="U59" s="34"/>
+      <c r="V59" s="34"/>
+      <c r="W59" s="34"/>
+      <c r="X59" s="24"/>
+      <c r="Y59" s="25"/>
+      <c r="Z59" s="25"/>
+      <c r="AA59" s="26"/>
+      <c r="AB59" s="35"/>
+      <c r="AC59" s="44"/>
+      <c r="AD59" s="52"/>
+    </row>
+    <row r="60" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D60" s="75"/>
+      <c r="E60" s="74"/>
+      <c r="F60" s="74"/>
+      <c r="G60" s="74"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="76"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="33"/>
+      <c r="P60" s="34"/>
+      <c r="Q60" s="34"/>
+      <c r="R60" s="34"/>
+      <c r="S60" s="34"/>
+      <c r="T60" s="34"/>
+      <c r="U60" s="34"/>
+      <c r="V60" s="34"/>
+      <c r="W60" s="34"/>
+      <c r="X60" s="24"/>
+      <c r="Y60" s="25"/>
+      <c r="Z60" s="25"/>
+      <c r="AA60" s="26"/>
+      <c r="AB60" s="35"/>
+      <c r="AC60" s="44"/>
+      <c r="AD60" s="52"/>
+    </row>
+    <row r="61" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D61" s="68"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="69"/>
+      <c r="I61" s="70"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="33"/>
+      <c r="P61" s="34"/>
+      <c r="Q61" s="34"/>
+      <c r="R61" s="34"/>
+      <c r="S61" s="34"/>
+      <c r="T61" s="34"/>
+      <c r="U61" s="34"/>
+      <c r="V61" s="34"/>
+      <c r="W61" s="34"/>
+      <c r="X61" s="27"/>
+      <c r="Y61" s="28"/>
+      <c r="Z61" s="28"/>
+      <c r="AA61" s="29"/>
+      <c r="AB61" s="35"/>
+      <c r="AC61" s="44"/>
+      <c r="AD61" s="52"/>
+    </row>
+    <row r="62" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="D62" s="71"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="72"/>
+      <c r="G62" s="72"/>
+      <c r="H62" s="72"/>
+      <c r="I62" s="73"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="43"/>
+      <c r="O62" s="36"/>
+      <c r="P62" s="37"/>
+      <c r="Q62" s="37"/>
+      <c r="R62" s="37"/>
+      <c r="S62" s="37"/>
+      <c r="T62" s="37"/>
+      <c r="U62" s="37"/>
+      <c r="V62" s="37"/>
+      <c r="W62" s="37"/>
+      <c r="X62" s="37"/>
+      <c r="Y62" s="37"/>
+      <c r="Z62" s="37"/>
+      <c r="AA62" s="37"/>
+      <c r="AB62" s="38"/>
+      <c r="AC62" s="44"/>
+      <c r="AD62" s="52"/>
+    </row>
+    <row r="63" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M63" s="51"/>
+      <c r="N63" s="45"/>
+      <c r="O63" s="46"/>
+      <c r="P63" s="46"/>
+      <c r="Q63" s="46"/>
+      <c r="R63" s="46"/>
+      <c r="S63" s="46"/>
+      <c r="T63" s="46"/>
+      <c r="U63" s="46"/>
+      <c r="V63" s="46"/>
+      <c r="W63" s="46"/>
+      <c r="X63" s="46"/>
+      <c r="Y63" s="46"/>
+      <c r="Z63" s="46"/>
+      <c r="AA63" s="46"/>
+      <c r="AB63" s="46"/>
+      <c r="AC63" s="47"/>
+      <c r="AD63" s="52"/>
+    </row>
+    <row r="64" spans="4:30" x14ac:dyDescent="0.35">
+      <c r="M64" s="53"/>
+      <c r="N64" s="54"/>
+      <c r="O64" s="54"/>
+      <c r="P64" s="54"/>
+      <c r="Q64" s="54"/>
+      <c r="R64" s="54"/>
+      <c r="S64" s="54"/>
+      <c r="T64" s="54"/>
+      <c r="U64" s="54"/>
+      <c r="V64" s="54"/>
+      <c r="W64" s="54"/>
+      <c r="X64" s="54"/>
+      <c r="Y64" s="54"/>
+      <c r="Z64" s="54"/>
+      <c r="AA64" s="54"/>
+      <c r="AB64" s="54"/>
+      <c r="AC64" s="54"/>
+      <c r="AD64" s="55"/>
+    </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="D60:I60"/>
+    <mergeCell ref="D42:I42"/>
+    <mergeCell ref="D50:I50"/>
+    <mergeCell ref="D52:I52"/>
+    <mergeCell ref="D53:I53"/>
+    <mergeCell ref="P55:U55"/>
+    <mergeCell ref="D57:I57"/>
+    <mergeCell ref="D35:I35"/>
+    <mergeCell ref="D32:I32"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="P37:U37"/>
+    <mergeCell ref="D39:I39"/>
+    <mergeCell ref="D41:I41"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>